<commit_message>
Optimizations w/ 500 evaluations
</commit_message>
<xml_diff>
--- a/analysis/output_2021-05-18_21-50-51.xlsx
+++ b/analysis/output_2021-05-18_21-50-51.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephan/Documents/GitHub/2_183_TermProj/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ED86B4-4694-964F-8DF0-8FE908DDE213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421CCB4-28D3-EC43-A80B-C3D82338F8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,7 +390,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48A33740-0308-2A42-AA52-D54837AF58A1}" name="Table1" displayName="Table1" ref="A1:O66" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:O66" xr:uid="{D154B5F9-CD93-1A4F-A398-473136EA146F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O66">
-    <sortCondition ref="C1:C66"/>
+    <sortCondition ref="L1:L66"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{E64D41E8-BB1E-8E44-8016-2F8A315EDD58}" name="Simulation" dataDxfId="5"/>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O48" sqref="B48:O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -789,51 +789,51 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>10.906222325661885</v>
+        <v>3.4000339721819084</v>
       </c>
       <c r="C2">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.0937776743381153</v>
+        <v>10.599966027818091</v>
       </c>
       <c r="D2" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22098411959557968</v>
+        <v>0.75714043055843505</v>
       </c>
       <c r="E2">
-        <v>0.92700212797616766</v>
+        <v>2.3563215470535948</v>
       </c>
       <c r="F2">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.14160212797616767</v>
+        <v>-1.2154705359490592E-4</v>
       </c>
       <c r="G2">
-        <v>-27.400718568693037</v>
+        <v>-2.8961799755479558</v>
       </c>
       <c r="H2">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-22.599281431306963</v>
+        <v>-47.103820024452041</v>
       </c>
       <c r="I2" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.45198562862613928</v>
+        <v>0.94207640048904084</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2">
         <v>1.5708</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M2">
         <v>14</v>
       </c>
       <c r="N2">
-        <v>0.78539999999999999</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O2">
         <v>-50</v>
@@ -841,36 +841,36 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B3">
-        <v>10.906222325661885</v>
+        <v>2.744578901867996</v>
       </c>
       <c r="C3">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.0937776743381153</v>
+        <v>11.255421098132004</v>
       </c>
       <c r="D3" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22098411959557968</v>
+        <v>0.80395864986657173</v>
       </c>
       <c r="E3">
-        <v>0.92700212797616766</v>
+        <v>0.80803646616466207</v>
       </c>
       <c r="F3">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.14160212797616767</v>
+        <v>-2.2636466164662084E-2</v>
       </c>
       <c r="G3">
-        <v>-27.400718568693037</v>
+        <v>-10.201235887648528</v>
       </c>
       <c r="H3">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-22.599281431306963</v>
+        <v>-39.798764112351471</v>
       </c>
       <c r="I3" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.45198562862613928</v>
+        <v>0.7959752822470294</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -879,7 +879,7 @@
         <v>1.5708</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M3">
         <v>14</v>
@@ -893,51 +893,51 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>10.906222325661885</v>
+        <v>2.5142693426197287</v>
       </c>
       <c r="C4">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.0937776743381153</v>
+        <v>11.485730657380271</v>
       </c>
       <c r="D4" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22098411959557968</v>
+        <v>0.82040933267001936</v>
       </c>
       <c r="E4">
-        <v>0.92700212797616766</v>
+        <v>0.78509778249465201</v>
       </c>
       <c r="F4">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.92700212797616766</v>
+        <v>3.022175053479792E-4</v>
       </c>
       <c r="G4">
-        <v>-27.400718568693037</v>
+        <v>-5.8806851197080983</v>
       </c>
       <c r="H4">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-22.599281431306963</v>
+        <v>-44.119314880291903</v>
       </c>
       <c r="I4" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.45198562862613928</v>
+        <v>0.88238629760583809</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <v>1.5708</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M4">
         <v>14</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O4">
         <v>-50</v>
@@ -945,45 +945,45 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>10.906222325661885</v>
+        <v>0.60485634565557433</v>
       </c>
       <c r="C5">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.0937776743381153</v>
+        <v>13.395143654344425</v>
       </c>
       <c r="D5" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22098411959557968</v>
+        <v>0.95679597531031602</v>
       </c>
       <c r="E5">
-        <v>0.92700212797616766</v>
+        <v>1.5710418429033823</v>
       </c>
       <c r="F5">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0.64379787202383232</v>
+        <v>-2.4184290338236103E-4</v>
       </c>
       <c r="G5">
-        <v>-27.400718568693037</v>
+        <v>-1.1473067014842466</v>
       </c>
       <c r="H5">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-22.599281431306963</v>
+        <v>-48.852693298515753</v>
       </c>
       <c r="I5" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.45198562862613928</v>
+        <v>0.97705386597031507</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <v>1.5708</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M5">
         <v>14</v>
@@ -997,36 +997,36 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B6">
-        <v>10.906222325661885</v>
+        <v>0.5430226005706229</v>
       </c>
       <c r="C6">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.0937776743381153</v>
+        <v>13.456977399429377</v>
       </c>
       <c r="D6" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22098411959557968</v>
+        <v>0.96121267138781263</v>
       </c>
       <c r="E6">
-        <v>0.92700212797616766</v>
+        <v>1.1904643963441685E-4</v>
       </c>
       <c r="F6">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>1.4291978720238321</v>
+        <v>-1.1904643963441685E-4</v>
       </c>
       <c r="G6">
-        <v>-27.400718568693037</v>
+        <v>0.19305650313308748</v>
       </c>
       <c r="H6">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-22.599281431306963</v>
+        <v>-50.193056503133086</v>
       </c>
       <c r="I6" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.45198562862613928</v>
+        <v>1.0038611300626616</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -1035,13 +1035,13 @@
         <v>1.5708</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M6">
         <v>14</v>
       </c>
       <c r="N6">
-        <v>2.3561999999999999</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <v>-50</v>
@@ -1049,51 +1049,51 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B7">
-        <v>10.878022238210846</v>
+        <v>0.22599794935528578</v>
       </c>
       <c r="C7">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.1219777617891538</v>
+        <v>13.774002050644715</v>
       </c>
       <c r="D7" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22299841155636813</v>
+        <v>0.98385728933176531</v>
       </c>
       <c r="E7">
-        <v>0.96136258085305115</v>
+        <v>1.570281885757705</v>
       </c>
       <c r="F7">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.96136258085305115</v>
+        <v>5.1811424229497582E-4</v>
       </c>
       <c r="G7">
-        <v>-26.250818497465005</v>
+        <v>-0.88538910829364359</v>
       </c>
       <c r="H7">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-23.749181502534995</v>
+        <v>-49.114610891706356</v>
       </c>
       <c r="I7" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.47498363005069988</v>
+        <v>0.98229221783412712</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
       <c r="K7">
-        <v>3.1415999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M7">
         <v>14</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1.5708</v>
       </c>
       <c r="O7">
         <v>-50</v>
@@ -1101,51 +1101,51 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B8">
-        <v>10.784411086079967</v>
+        <v>2.1593038339367231E-2</v>
       </c>
       <c r="C8">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.2155889139200333</v>
+        <v>13.978406961660633</v>
       </c>
       <c r="D8" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22968492242285951</v>
+        <v>0.99845764011861671</v>
       </c>
       <c r="E8">
-        <v>0.85219625583050651</v>
+        <v>2.3355974509498942</v>
       </c>
       <c r="F8">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-6.6796255830506523E-2</v>
+        <v>2.0602549050105612E-2</v>
       </c>
       <c r="G8">
-        <v>-23.770343001701715</v>
+        <v>-0.3560193649975919</v>
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.229656998298285</v>
+        <v>-49.643980635002407</v>
       </c>
       <c r="I8" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.52459313996596568</v>
+        <v>0.9928796127000481</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K8">
         <v>1.5708</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M8">
         <v>14</v>
       </c>
       <c r="N8">
-        <v>0.78539999999999999</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O8">
         <v>-50</v>
@@ -1153,36 +1153,36 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>10.784411086079967</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.2155889139200333</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22968492242285951</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.85219625583050651</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-6.6796255830506523E-2</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>-23.770343001701715</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.229656998298285</v>
+        <v>-50</v>
       </c>
       <c r="I9" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.52459313996596568</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -1191,13 +1191,13 @@
         <v>1.5708</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M9">
         <v>14</v>
       </c>
       <c r="N9">
-        <v>0.78539999999999999</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>-50</v>
@@ -1205,36 +1205,36 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>10.784411086079967</v>
+        <v>10.499308160078709</v>
       </c>
       <c r="C10">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.2155889139200333</v>
+        <v>3.5006918399212914</v>
       </c>
       <c r="D10" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22968492242285951</v>
+        <v>0.25004941713723511</v>
       </c>
       <c r="E10">
-        <v>0.85219625583050651</v>
+        <v>0.89441113446496479</v>
       </c>
       <c r="F10">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.85219625583050651</v>
+        <v>-0.1090111344649648</v>
       </c>
       <c r="G10">
-        <v>-23.770343001701715</v>
+        <v>-24.439339774013547</v>
       </c>
       <c r="H10">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.229656998298285</v>
+        <v>-25.560660225986453</v>
       </c>
       <c r="I10" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.52459313996596568</v>
+        <v>0.51121320451972907</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -1243,13 +1243,13 @@
         <v>1.5708</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="M10">
         <v>14</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O10">
         <v>-50</v>
@@ -1257,51 +1257,51 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B11">
-        <v>10.784411086079967</v>
+        <v>8.7733038156135592</v>
       </c>
       <c r="C11">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.2155889139200333</v>
+        <v>5.2266961843864408</v>
       </c>
       <c r="D11" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22968492242285951</v>
+        <v>0.37333544174188865</v>
       </c>
       <c r="E11">
-        <v>0.85219625583050651</v>
+        <v>0.888026506772012</v>
       </c>
       <c r="F11">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0.71860374416949346</v>
+        <v>-0.10262650677201202</v>
       </c>
       <c r="G11">
-        <v>-23.770343001701715</v>
+        <v>-31.326856659645902</v>
       </c>
       <c r="H11">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.229656998298285</v>
+        <v>-18.673143340354098</v>
       </c>
       <c r="I11" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.52459313996596568</v>
+        <v>0.37346286680708196</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11">
         <v>1.5708</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="M11">
         <v>14</v>
       </c>
       <c r="N11">
-        <v>1.5708</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O11">
         <v>-50</v>
@@ -1309,36 +1309,36 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>10.784411086079967</v>
+        <v>7.9314641682638065</v>
       </c>
       <c r="C12">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.2155889139200333</v>
+        <v>6.0685358317361935</v>
       </c>
       <c r="D12" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.22968492242285951</v>
+        <v>0.43346684512401384</v>
       </c>
       <c r="E12">
-        <v>0.85219625583050651</v>
+        <v>0.41475828641032475</v>
       </c>
       <c r="F12">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>1.5040037441694933</v>
+        <v>-0.41475828641032475</v>
       </c>
       <c r="G12">
-        <v>-23.770343001701715</v>
+        <v>-17.901459927104511</v>
       </c>
       <c r="H12">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.229656998298285</v>
+        <v>-32.098540072895489</v>
       </c>
       <c r="I12" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.52459313996596568</v>
+        <v>0.64197080145790975</v>
       </c>
       <c r="J12">
         <v>2</v>
@@ -1347,13 +1347,13 @@
         <v>1.5708</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="M12">
         <v>14</v>
       </c>
       <c r="N12">
-        <v>2.3561999999999999</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>-50</v>
@@ -1361,51 +1361,51 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>10.585348818604754</v>
+        <v>7.8680847462490462</v>
       </c>
       <c r="C13">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.4146511813952465</v>
+        <v>6.1319152537509538</v>
       </c>
       <c r="D13" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.24390365581394619</v>
+        <v>0.43799394669649672</v>
       </c>
       <c r="E13">
-        <v>0.91317589587935233</v>
+        <v>0.35481923329909559</v>
       </c>
       <c r="F13">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.12777589587935234</v>
+        <v>-0.35481923329909559</v>
       </c>
       <c r="G13">
-        <v>-24.753182054066464</v>
+        <v>-16.87791579408179</v>
       </c>
       <c r="H13">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-25.246817945933536</v>
+        <v>-33.122084205918213</v>
       </c>
       <c r="I13" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.50493635891867072</v>
+        <v>0.66244168411836424</v>
       </c>
       <c r="J13">
         <v>2</v>
       </c>
       <c r="K13">
-        <v>1.5708</v>
+        <v>3.1415999999999999</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="M13">
         <v>14</v>
       </c>
       <c r="N13">
-        <v>0.78539999999999999</v>
+        <v>0</v>
       </c>
       <c r="O13">
         <v>-50</v>
@@ -1413,45 +1413,45 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B14">
-        <v>10.585348818604754</v>
+        <v>6.6592866623578741</v>
       </c>
       <c r="C14">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.4146511813952465</v>
+        <v>7.3407133376421259</v>
       </c>
       <c r="D14" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.24390365581394619</v>
+        <v>0.52433666697443759</v>
       </c>
       <c r="E14">
-        <v>0.91317589587935233</v>
+        <v>0.33923882984389042</v>
       </c>
       <c r="F14">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.91317589587935233</v>
+        <v>-0.33923882984389042</v>
       </c>
       <c r="G14">
-        <v>-24.753182054066464</v>
+        <v>-23.46730562987506</v>
       </c>
       <c r="H14">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-25.246817945933536</v>
+        <v>-26.53269437012494</v>
       </c>
       <c r="I14" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.50493635891867072</v>
+        <v>0.53065388740249875</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14">
         <v>1.5708</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="M14">
         <v>14</v>
@@ -1465,51 +1465,51 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="B15">
-        <v>10.585348818604754</v>
+        <v>6.3743981072779015</v>
       </c>
       <c r="C15">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.4146511813952465</v>
+        <v>7.6256018927220985</v>
       </c>
       <c r="D15" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.24390365581394619</v>
+        <v>0.54468584948014986</v>
       </c>
       <c r="E15">
-        <v>0.91317589587935233</v>
+        <v>0.30915273724810233</v>
       </c>
       <c r="F15">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0.65762410412064765</v>
+        <v>-0.30915273724810233</v>
       </c>
       <c r="G15">
-        <v>-24.753182054066464</v>
+        <v>-22.557797164235772</v>
       </c>
       <c r="H15">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-25.246817945933536</v>
+        <v>-27.442202835764228</v>
       </c>
       <c r="I15" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.50493635891867072</v>
+        <v>0.54884405671528458</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K15">
-        <v>1.5708</v>
+        <v>3.1415999999999999</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="M15">
         <v>14</v>
       </c>
       <c r="N15">
-        <v>1.5708</v>
+        <v>0</v>
       </c>
       <c r="O15">
         <v>-50</v>
@@ -1517,36 +1517,36 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>10.585348818604754</v>
+        <v>5.043608780281355</v>
       </c>
       <c r="C16">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.4146511813952465</v>
+        <v>8.956391219718645</v>
       </c>
       <c r="D16" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.24390365581394619</v>
+        <v>0.63974222997990327</v>
       </c>
       <c r="E16">
-        <v>0.91317589587935233</v>
+        <v>1.6178626419664945</v>
       </c>
       <c r="F16">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>1.4430241041206475</v>
+        <v>-4.7062641966494567E-2</v>
       </c>
       <c r="G16">
-        <v>-24.753182054066464</v>
+        <v>-17.920526461740312</v>
       </c>
       <c r="H16">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-25.246817945933536</v>
+        <v>-32.079473538259691</v>
       </c>
       <c r="I16" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.50493635891867072</v>
+        <v>0.64158947076519379</v>
       </c>
       <c r="J16">
         <v>2</v>
@@ -1555,13 +1555,13 @@
         <v>1.5708</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="M16">
         <v>14</v>
       </c>
       <c r="N16">
-        <v>2.3561999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="O16">
         <v>-50</v>
@@ -1569,51 +1569,51 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B17">
-        <v>10.552836725047491</v>
+        <v>4.4932513513810193</v>
       </c>
       <c r="C17">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.4471632749525085</v>
+        <v>9.5067486486189807</v>
       </c>
       <c r="D17" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.24622594821089347</v>
+        <v>0.67905347490135581</v>
       </c>
       <c r="E17">
-        <v>1.0891326578930076</v>
+        <v>1.4973105497117114</v>
       </c>
       <c r="F17">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-1.0891326578930076</v>
+        <v>7.3489450288288571E-2</v>
       </c>
       <c r="G17">
-        <v>-29.429198612896048</v>
+        <v>-23.551161455515949</v>
       </c>
       <c r="H17">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-20.570801387103952</v>
+        <v>-26.448838544484051</v>
       </c>
       <c r="I17" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.41141602774207903</v>
+        <v>0.52897677088968098</v>
       </c>
       <c r="J17">
         <v>3</v>
       </c>
       <c r="K17">
-        <v>3.1415999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="M17">
         <v>14</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1.5708</v>
       </c>
       <c r="O17">
         <v>-50</v>
@@ -1621,39 +1621,39 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B18">
-        <v>10.499308160078709</v>
+        <v>3.335356272803502</v>
       </c>
       <c r="C18">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.5006918399212914</v>
+        <v>10.664643727196498</v>
       </c>
       <c r="D18" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.25004941713723511</v>
+        <v>0.76176026622832127</v>
       </c>
       <c r="E18">
-        <v>0.89441113446496479</v>
+        <v>2.3590384677248712</v>
       </c>
       <c r="F18">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.1090111344649648</v>
+        <v>-2.8384677248713963E-3</v>
       </c>
       <c r="G18">
-        <v>-24.439339774013547</v>
+        <v>-17.639696982700809</v>
       </c>
       <c r="H18">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-25.560660225986453</v>
+        <v>-32.360303017299188</v>
       </c>
       <c r="I18" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.51121320451972907</v>
+        <v>0.64720606034598371</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K18">
         <v>1.5708</v>
@@ -1665,7 +1665,7 @@
         <v>14</v>
       </c>
       <c r="N18">
-        <v>0.78539999999999999</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O18">
         <v>-50</v>
@@ -1673,36 +1673,36 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B19">
-        <v>10.499308160078709</v>
+        <v>2.401507748371428</v>
       </c>
       <c r="C19">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.5006918399212914</v>
+        <v>11.598492251628572</v>
       </c>
       <c r="D19" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.25004941713723511</v>
+        <v>0.82846373225918379</v>
       </c>
       <c r="E19">
-        <v>0.89441113446496479</v>
+        <v>2.5655023310780454</v>
       </c>
       <c r="F19">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.1090111344649648</v>
+        <v>-0.20930233107804552</v>
       </c>
       <c r="G19">
-        <v>-24.439339774013547</v>
+        <v>-2.191225676254779</v>
       </c>
       <c r="H19">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-25.560660225986453</v>
+        <v>-47.808774323745219</v>
       </c>
       <c r="I19" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.51121320451972907</v>
+        <v>0.95617548647490436</v>
       </c>
       <c r="J19">
         <v>2</v>
@@ -1711,13 +1711,13 @@
         <v>1.5708</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M19">
         <v>14</v>
       </c>
       <c r="N19">
-        <v>0.78539999999999999</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O19">
         <v>-50</v>
@@ -1725,51 +1725,51 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>10.439491785779056</v>
+        <v>9.6952011832242739</v>
       </c>
       <c r="C20">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.5605082142209437</v>
+        <v>4.3047988167757261</v>
       </c>
       <c r="D20" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.25432201530149595</v>
+        <v>0.30748562976969473</v>
       </c>
       <c r="E20">
-        <v>0.9160244752894342</v>
+        <v>0.99191197972707457</v>
       </c>
       <c r="F20">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.9160244752894342</v>
+        <v>-0.20651197972707458</v>
       </c>
       <c r="G20">
-        <v>-22.754223446492428</v>
+        <v>-25.204976240742688</v>
       </c>
       <c r="H20">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-27.245776553507572</v>
+        <v>-24.795023759257312</v>
       </c>
       <c r="I20" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.54491553107015145</v>
+        <v>0.49590047518514624</v>
       </c>
       <c r="J20">
         <v>2</v>
       </c>
       <c r="K20">
-        <v>3.1415999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M20">
         <v>14</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O20">
         <v>-50</v>
@@ -1777,45 +1777,45 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>10.357264128043649</v>
+        <v>9.6952011832242739</v>
       </c>
       <c r="C21">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.6427358719563507</v>
+        <v>4.3047988167757261</v>
       </c>
       <c r="D21" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.2601954194254536</v>
+        <v>0.30748562976969473</v>
       </c>
       <c r="E21">
-        <v>1.0156881149436505</v>
+        <v>0.99191197972707457</v>
       </c>
       <c r="F21">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-1.0156881149436505</v>
+        <v>-0.99191197972707457</v>
       </c>
       <c r="G21">
-        <v>-24.689535971972997</v>
+        <v>-25.204976240742688</v>
       </c>
       <c r="H21">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-25.310464028027003</v>
+        <v>-24.795023759257312</v>
       </c>
       <c r="I21" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.50620928056054004</v>
+        <v>0.49590047518514624</v>
       </c>
       <c r="J21">
         <v>2</v>
       </c>
       <c r="K21">
-        <v>3.1415999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M21">
         <v>14</v>
@@ -1829,51 +1829,51 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>10.352459970417151</v>
+        <v>9.6952011832242739</v>
       </c>
       <c r="C22">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.6475400295828493</v>
+        <v>4.3047988167757261</v>
       </c>
       <c r="D22" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.26053857354163207</v>
+        <v>0.30748562976969473</v>
       </c>
       <c r="E22">
-        <v>1.0503872048170404</v>
+        <v>0.99191197972707457</v>
       </c>
       <c r="F22">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.26498720481704041</v>
+        <v>0.57888802027292541</v>
       </c>
       <c r="G22">
-        <v>-31.214827041527919</v>
+        <v>-25.204976240742688</v>
       </c>
       <c r="H22">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.785172958472081</v>
+        <v>-24.795023759257312</v>
       </c>
       <c r="I22" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.37570345916944164</v>
+        <v>0.49590047518514624</v>
       </c>
       <c r="J22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K22">
         <v>1.5708</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M22">
         <v>14</v>
       </c>
       <c r="N22">
-        <v>0.78539999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="O22">
         <v>-50</v>
@@ -1881,51 +1881,51 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B23">
-        <v>10.352459970417151</v>
+        <v>9.6952011832242739</v>
       </c>
       <c r="C23">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.6475400295828493</v>
+        <v>4.3047988167757261</v>
       </c>
       <c r="D23" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.26053857354163207</v>
+        <v>0.30748562976969473</v>
       </c>
       <c r="E23">
-        <v>1.0503872048170404</v>
+        <v>0.99191197972707457</v>
       </c>
       <c r="F23">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-1.0503872048170404</v>
+        <v>1.3642880202729253</v>
       </c>
       <c r="G23">
-        <v>-31.214827041527919</v>
+        <v>-25.204976240742688</v>
       </c>
       <c r="H23">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.785172958472081</v>
+        <v>-24.795023759257312</v>
       </c>
       <c r="I23" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.37570345916944164</v>
+        <v>0.49590047518514624</v>
       </c>
       <c r="J23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K23">
         <v>1.5708</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M23">
         <v>14</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O23">
         <v>-50</v>
@@ -1933,36 +1933,36 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B24">
-        <v>10.352459970417151</v>
+        <v>9.3773039027020957</v>
       </c>
       <c r="C24">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.6475400295828493</v>
+        <v>4.6226960972979043</v>
       </c>
       <c r="D24" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.26053857354163207</v>
+        <v>0.33019257837842175</v>
       </c>
       <c r="E24">
-        <v>1.0503872048170404</v>
+        <v>0.98464320372739678</v>
       </c>
       <c r="F24">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0.52041279518295958</v>
+        <v>-0.19924320372739679</v>
       </c>
       <c r="G24">
-        <v>-31.214827041527919</v>
+        <v>-31.735073786144124</v>
       </c>
       <c r="H24">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.785172958472081</v>
+        <v>-18.264926213855876</v>
       </c>
       <c r="I24" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.37570345916944164</v>
+        <v>0.36529852427711751</v>
       </c>
       <c r="J24">
         <v>3</v>
@@ -1971,13 +1971,13 @@
         <v>1.5708</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M24">
         <v>14</v>
       </c>
       <c r="N24">
-        <v>1.5708</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O24">
         <v>-50</v>
@@ -1985,36 +1985,36 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B25">
-        <v>10.352459970417151</v>
+        <v>9.3773039027020957</v>
       </c>
       <c r="C25">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.6475400295828493</v>
+        <v>4.6226960972979043</v>
       </c>
       <c r="D25" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.26053857354163207</v>
+        <v>0.33019257837842175</v>
       </c>
       <c r="E25">
-        <v>1.0503872048170404</v>
+        <v>0.98464320372739678</v>
       </c>
       <c r="F25">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>1.3058127951829595</v>
+        <v>-0.98464320372739678</v>
       </c>
       <c r="G25">
-        <v>-31.214827041527919</v>
+        <v>-31.735073786144124</v>
       </c>
       <c r="H25">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.785172958472081</v>
+        <v>-18.264926213855876</v>
       </c>
       <c r="I25" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.37570345916944164</v>
+        <v>0.36529852427711751</v>
       </c>
       <c r="J25">
         <v>3</v>
@@ -2023,13 +2023,13 @@
         <v>1.5708</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M25">
         <v>14</v>
       </c>
       <c r="N25">
-        <v>2.3561999999999999</v>
+        <v>0</v>
       </c>
       <c r="O25">
         <v>-50</v>
@@ -2037,36 +2037,36 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26">
-        <v>10.125292754787109</v>
+        <v>9.3773039027020957</v>
       </c>
       <c r="C26">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>3.8747072452128908</v>
+        <v>4.6226960972979043</v>
       </c>
       <c r="D26" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.27676480322949221</v>
+        <v>0.33019257837842175</v>
       </c>
       <c r="E26">
-        <v>0.94899438432264316</v>
+        <v>0.98464320372739678</v>
       </c>
       <c r="F26">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.16359438432264317</v>
+        <v>0.5861567962726032</v>
       </c>
       <c r="G26">
-        <v>-30.869370476054289</v>
+        <v>-31.735073786144124</v>
       </c>
       <c r="H26">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-19.130629523945711</v>
+        <v>-18.264926213855876</v>
       </c>
       <c r="I26" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.38261259047891422</v>
+        <v>0.36529852427711751</v>
       </c>
       <c r="J26">
         <v>3</v>
@@ -2075,13 +2075,13 @@
         <v>1.5708</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M26">
         <v>14</v>
       </c>
       <c r="N26">
-        <v>0.78539999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="O26">
         <v>-50</v>
@@ -2089,39 +2089,39 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B27">
-        <v>9.6952011832242739</v>
+        <v>9.3773039027020957</v>
       </c>
       <c r="C27">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.3047988167757261</v>
+        <v>4.6226960972979043</v>
       </c>
       <c r="D27" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.30748562976969473</v>
+        <v>0.33019257837842175</v>
       </c>
       <c r="E27">
-        <v>0.99191197972707457</v>
+        <v>0.98464320372739678</v>
       </c>
       <c r="F27">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.20651197972707458</v>
+        <v>1.371556796272603</v>
       </c>
       <c r="G27">
-        <v>-25.204976240742688</v>
+        <v>-31.735073786144124</v>
       </c>
       <c r="H27">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-24.795023759257312</v>
+        <v>-18.264926213855876</v>
       </c>
       <c r="I27" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.49590047518514624</v>
+        <v>0.36529852427711751</v>
       </c>
       <c r="J27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27">
         <v>1.5708</v>
@@ -2133,7 +2133,7 @@
         <v>14</v>
       </c>
       <c r="N27">
-        <v>0.78539999999999999</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O27">
         <v>-50</v>
@@ -2141,51 +2141,51 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="B28">
-        <v>9.6952011832242739</v>
+        <v>10.906222325661885</v>
       </c>
       <c r="C28">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.3047988167757261</v>
+        <v>3.0937776743381153</v>
       </c>
       <c r="D28" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.30748562976969473</v>
+        <v>0.22098411959557968</v>
       </c>
       <c r="E28">
-        <v>0.99191197972707457</v>
+        <v>0.92700212797616766</v>
       </c>
       <c r="F28">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.99191197972707457</v>
+        <v>-0.14160212797616767</v>
       </c>
       <c r="G28">
-        <v>-25.204976240742688</v>
+        <v>-27.400718568693037</v>
       </c>
       <c r="H28">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-24.795023759257312</v>
+        <v>-22.599281431306963</v>
       </c>
       <c r="I28" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.49590047518514624</v>
+        <v>0.45198562862613928</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K28">
         <v>1.5708</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M28">
         <v>14</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O28">
         <v>-50</v>
@@ -2193,51 +2193,51 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B29">
-        <v>9.6952011832242739</v>
+        <v>10.906222325661885</v>
       </c>
       <c r="C29">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.3047988167757261</v>
+        <v>3.0937776743381153</v>
       </c>
       <c r="D29" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.30748562976969473</v>
+        <v>0.22098411959557968</v>
       </c>
       <c r="E29">
-        <v>0.99191197972707457</v>
+        <v>0.92700212797616766</v>
       </c>
       <c r="F29">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0.57888802027292541</v>
+        <v>-0.92700212797616766</v>
       </c>
       <c r="G29">
-        <v>-25.204976240742688</v>
+        <v>-27.400718568693037</v>
       </c>
       <c r="H29">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-24.795023759257312</v>
+        <v>-22.599281431306963</v>
       </c>
       <c r="I29" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.49590047518514624</v>
+        <v>0.45198562862613928</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K29">
         <v>1.5708</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M29">
         <v>14</v>
       </c>
       <c r="N29">
-        <v>1.5708</v>
+        <v>0</v>
       </c>
       <c r="O29">
         <v>-50</v>
@@ -2245,51 +2245,51 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B30">
-        <v>9.6952011832242739</v>
+        <v>10.906222325661885</v>
       </c>
       <c r="C30">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.3047988167757261</v>
+        <v>3.0937776743381153</v>
       </c>
       <c r="D30" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.30748562976969473</v>
+        <v>0.22098411959557968</v>
       </c>
       <c r="E30">
-        <v>0.99191197972707457</v>
+        <v>0.92700212797616766</v>
       </c>
       <c r="F30">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>1.3642880202729253</v>
+        <v>0.64379787202383232</v>
       </c>
       <c r="G30">
-        <v>-25.204976240742688</v>
+        <v>-27.400718568693037</v>
       </c>
       <c r="H30">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-24.795023759257312</v>
+        <v>-22.599281431306963</v>
       </c>
       <c r="I30" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.49590047518514624</v>
+        <v>0.45198562862613928</v>
       </c>
       <c r="J30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K30">
         <v>1.5708</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M30">
         <v>14</v>
       </c>
       <c r="N30">
-        <v>2.3561999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="O30">
         <v>-50</v>
@@ -2297,51 +2297,51 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B31">
-        <v>9.6783889588051313</v>
+        <v>10.906222325661885</v>
       </c>
       <c r="C31">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.3216110411948687</v>
+        <v>3.0937776743381153</v>
       </c>
       <c r="D31" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.30868650294249061</v>
+        <v>0.22098411959557968</v>
       </c>
       <c r="E31">
-        <v>0.63668707506666289</v>
+        <v>0.92700212797616766</v>
       </c>
       <c r="F31">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.63668707506666289</v>
+        <v>1.4291978720238321</v>
       </c>
       <c r="G31">
-        <v>-20.806605765438739</v>
+        <v>-27.400718568693037</v>
       </c>
       <c r="H31">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-29.193394234561261</v>
+        <v>-22.599281431306963</v>
       </c>
       <c r="I31" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.58386788469122519</v>
+        <v>0.45198562862613928</v>
       </c>
       <c r="J31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K31">
         <v>1.5708</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M31">
         <v>14</v>
       </c>
       <c r="N31">
-        <v>0</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O31">
         <v>-50</v>
@@ -2349,45 +2349,45 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B32">
-        <v>9.5564130488735231</v>
+        <v>10.878022238210846</v>
       </c>
       <c r="C32">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.4435869511264769</v>
+        <v>3.1219777617891538</v>
       </c>
       <c r="D32" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.31739906793760547</v>
+        <v>0.22299841155636813</v>
       </c>
       <c r="E32">
-        <v>0.62560324580990911</v>
+        <v>0.96136258085305115</v>
       </c>
       <c r="F32">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.62560324580990911</v>
+        <v>-0.96136258085305115</v>
       </c>
       <c r="G32">
-        <v>-19.474191154986151</v>
+        <v>-26.250818497465005</v>
       </c>
       <c r="H32">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-30.525808845013849</v>
+        <v>-23.749181502534995</v>
       </c>
       <c r="I32" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.61051617690027693</v>
+        <v>0.47498363005069988</v>
       </c>
       <c r="J32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K32">
         <v>3.1415999999999999</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M32">
         <v>14</v>
@@ -2401,45 +2401,45 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B33">
-        <v>9.3773039027020957</v>
+        <v>10.784411086079967</v>
       </c>
       <c r="C33">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.6226960972979043</v>
+        <v>3.2155889139200333</v>
       </c>
       <c r="D33" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.33019257837842175</v>
+        <v>0.22968492242285951</v>
       </c>
       <c r="E33">
-        <v>0.98464320372739678</v>
+        <v>0.85219625583050651</v>
       </c>
       <c r="F33">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.19924320372739679</v>
+        <v>-6.6796255830506523E-2</v>
       </c>
       <c r="G33">
-        <v>-31.735073786144124</v>
+        <v>-23.770343001701715</v>
       </c>
       <c r="H33">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.264926213855876</v>
+        <v>-26.229656998298285</v>
       </c>
       <c r="I33" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.36529852427711751</v>
+        <v>0.52459313996596568</v>
       </c>
       <c r="J33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K33">
         <v>1.5708</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M33">
         <v>14</v>
@@ -2453,45 +2453,45 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B34">
-        <v>9.3773039027020957</v>
+        <v>10.784411086079967</v>
       </c>
       <c r="C34">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.6226960972979043</v>
+        <v>3.2155889139200333</v>
       </c>
       <c r="D34" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.33019257837842175</v>
+        <v>0.22968492242285951</v>
       </c>
       <c r="E34">
-        <v>0.98464320372739678</v>
+        <v>0.85219625583050651</v>
       </c>
       <c r="F34">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.98464320372739678</v>
+        <v>-0.85219625583050651</v>
       </c>
       <c r="G34">
-        <v>-31.735073786144124</v>
+        <v>-23.770343001701715</v>
       </c>
       <c r="H34">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.264926213855876</v>
+        <v>-26.229656998298285</v>
       </c>
       <c r="I34" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.36529852427711751</v>
+        <v>0.52459313996596568</v>
       </c>
       <c r="J34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K34">
         <v>1.5708</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M34">
         <v>14</v>
@@ -2505,45 +2505,45 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B35">
-        <v>9.3773039027020957</v>
+        <v>10.784411086079967</v>
       </c>
       <c r="C35">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.6226960972979043</v>
+        <v>3.2155889139200333</v>
       </c>
       <c r="D35" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.33019257837842175</v>
+        <v>0.22968492242285951</v>
       </c>
       <c r="E35">
-        <v>0.98464320372739678</v>
+        <v>0.85219625583050651</v>
       </c>
       <c r="F35">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0.5861567962726032</v>
+        <v>0.71860374416949346</v>
       </c>
       <c r="G35">
-        <v>-31.735073786144124</v>
+        <v>-23.770343001701715</v>
       </c>
       <c r="H35">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.264926213855876</v>
+        <v>-26.229656998298285</v>
       </c>
       <c r="I35" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.36529852427711751</v>
+        <v>0.52459313996596568</v>
       </c>
       <c r="J35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K35">
         <v>1.5708</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M35">
         <v>14</v>
@@ -2557,45 +2557,45 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B36">
-        <v>9.3773039027020957</v>
+        <v>10.784411086079967</v>
       </c>
       <c r="C36">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.6226960972979043</v>
+        <v>3.2155889139200333</v>
       </c>
       <c r="D36" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.33019257837842175</v>
+        <v>0.22968492242285951</v>
       </c>
       <c r="E36">
-        <v>0.98464320372739678</v>
+        <v>0.85219625583050651</v>
       </c>
       <c r="F36">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>1.371556796272603</v>
+        <v>1.5040037441694933</v>
       </c>
       <c r="G36">
-        <v>-31.735073786144124</v>
+        <v>-23.770343001701715</v>
       </c>
       <c r="H36">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.264926213855876</v>
+        <v>-26.229656998298285</v>
       </c>
       <c r="I36" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.36529852427711751</v>
+        <v>0.52459313996596568</v>
       </c>
       <c r="J36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K36">
         <v>1.5708</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="M36">
         <v>14</v>
@@ -2609,36 +2609,36 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B37">
-        <v>9.0978999796150344</v>
+        <v>10.439491785779056</v>
       </c>
       <c r="C37">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>4.9021000203849656</v>
+        <v>3.5605082142209437</v>
       </c>
       <c r="D37" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.35015000145606895</v>
+        <v>0.25432201530149595</v>
       </c>
       <c r="E37">
-        <v>0.40877579780980988</v>
+        <v>0.9160244752894342</v>
       </c>
       <c r="F37">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.40877579780980988</v>
+        <v>-0.9160244752894342</v>
       </c>
       <c r="G37">
-        <v>-15.950651249428327</v>
+        <v>-22.754223446492428</v>
       </c>
       <c r="H37">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-34.049348750571674</v>
+        <v>-27.245776553507572</v>
       </c>
       <c r="I37" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.68098697501143346</v>
+        <v>0.54491553107015145</v>
       </c>
       <c r="J37">
         <v>2</v>
@@ -2647,7 +2647,7 @@
         <v>3.1415999999999999</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M37">
         <v>14</v>
@@ -2661,36 +2661,36 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B38">
-        <v>8.7733038156135592</v>
+        <v>10.906222325661885</v>
       </c>
       <c r="C38">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>5.2266961843864408</v>
+        <v>3.0937776743381153</v>
       </c>
       <c r="D38" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.37333544174188865</v>
+        <v>0.22098411959557968</v>
       </c>
       <c r="E38">
-        <v>0.888026506772012</v>
+        <v>0.92700212797616766</v>
       </c>
       <c r="F38">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.10262650677201202</v>
+        <v>-0.14160212797616767</v>
       </c>
       <c r="G38">
-        <v>-31.326856659645902</v>
+        <v>-27.400718568693037</v>
       </c>
       <c r="H38">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-18.673143340354098</v>
+        <v>-22.599281431306963</v>
       </c>
       <c r="I38" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.37346286680708196</v>
+        <v>0.45198562862613928</v>
       </c>
       <c r="J38">
         <v>3</v>
@@ -2699,7 +2699,7 @@
         <v>1.5708</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M38">
         <v>14</v>
@@ -2713,42 +2713,42 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="B39">
-        <v>8.4839846910322265</v>
+        <v>10.784411086079967</v>
       </c>
       <c r="C39">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>5.5160153089677735</v>
+        <v>3.2155889139200333</v>
       </c>
       <c r="D39" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.39400109349769813</v>
+        <v>0.22968492242285951</v>
       </c>
       <c r="E39">
-        <v>0.34664534828490284</v>
+        <v>0.85219625583050651</v>
       </c>
       <c r="F39">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.34664534828490284</v>
+        <v>-6.6796255830506523E-2</v>
       </c>
       <c r="G39">
-        <v>-22.444602839079195</v>
+        <v>-23.770343001701715</v>
       </c>
       <c r="H39">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-27.555397160920805</v>
+        <v>-26.229656998298285</v>
       </c>
       <c r="I39" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.55110794321841605</v>
+        <v>0.52459313996596568</v>
       </c>
       <c r="J39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K39">
-        <v>3.1415999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>76</v>
@@ -2757,7 +2757,7 @@
         <v>14</v>
       </c>
       <c r="N39">
-        <v>0</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O39">
         <v>-50</v>
@@ -2765,45 +2765,45 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B40">
-        <v>8.3886643956393581</v>
+        <v>9.0978999796150344</v>
       </c>
       <c r="C40">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>5.6113356043606419</v>
+        <v>4.9021000203849656</v>
       </c>
       <c r="D40" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.40080968602576011</v>
+        <v>0.35015000145606895</v>
       </c>
       <c r="E40">
-        <v>0.38018833531851759</v>
+        <v>0.40877579780980988</v>
       </c>
       <c r="F40">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.38018833531851759</v>
+        <v>-0.40877579780980988</v>
       </c>
       <c r="G40">
-        <v>-23.591162741785809</v>
+        <v>-15.950651249428327</v>
       </c>
       <c r="H40">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.408837258214191</v>
+        <v>-34.049348750571674</v>
       </c>
       <c r="I40" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.52817674516428381</v>
+        <v>0.68098697501143346</v>
       </c>
       <c r="J40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K40">
-        <v>1.5708</v>
+        <v>3.1415999999999999</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M40">
         <v>14</v>
@@ -2817,42 +2817,42 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B41">
-        <v>8.3886643956393581</v>
+        <v>8.4839846910322265</v>
       </c>
       <c r="C41">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>5.6113356043606419</v>
+        <v>5.5160153089677735</v>
       </c>
       <c r="D41" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.40080968602576011</v>
+        <v>0.39400109349769813</v>
       </c>
       <c r="E41">
-        <v>0.38018833531851759</v>
+        <v>0.34664534828490284</v>
       </c>
       <c r="F41">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.38018833531851759</v>
+        <v>-0.34664534828490284</v>
       </c>
       <c r="G41">
-        <v>-23.591162741785809</v>
+        <v>-22.444602839079195</v>
       </c>
       <c r="H41">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.408837258214191</v>
+        <v>-27.555397160920805</v>
       </c>
       <c r="I41" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.52817674516428381</v>
+        <v>0.55110794321841605</v>
       </c>
       <c r="J41">
         <v>3</v>
       </c>
       <c r="K41">
-        <v>1.5708</v>
+        <v>3.1415999999999999</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>76</v>
@@ -2869,39 +2869,39 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="B42">
-        <v>8.2152516219881768</v>
+        <v>8.3886643956393581</v>
       </c>
       <c r="C42">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>5.7847483780118232</v>
+        <v>5.6113356043606419</v>
       </c>
       <c r="D42" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.41319631271513024</v>
+        <v>0.40080968602576011</v>
       </c>
       <c r="E42">
-        <v>0.24880518611687549</v>
+        <v>0.38018833531851759</v>
       </c>
       <c r="F42">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.24880518611687549</v>
+        <v>-0.38018833531851759</v>
       </c>
       <c r="G42">
-        <v>-15.093488401944091</v>
+        <v>-23.591162741785809</v>
       </c>
       <c r="H42">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-34.906511598055907</v>
+        <v>-26.408837258214191</v>
       </c>
       <c r="I42" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.69813023196111812</v>
+        <v>0.52817674516428381</v>
       </c>
       <c r="J42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K42">
         <v>1.5708</v>
@@ -2921,36 +2921,36 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B43">
-        <v>7.9314641682638065</v>
+        <v>8.2152516219881768</v>
       </c>
       <c r="C43">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>6.0685358317361935</v>
+        <v>5.7847483780118232</v>
       </c>
       <c r="D43" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.43346684512401384</v>
+        <v>0.41319631271513024</v>
       </c>
       <c r="E43">
-        <v>0.41475828641032475</v>
+        <v>0.24880518611687549</v>
       </c>
       <c r="F43">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.41475828641032475</v>
+        <v>-0.24880518611687549</v>
       </c>
       <c r="G43">
-        <v>-17.901459927104511</v>
+        <v>-15.093488401944091</v>
       </c>
       <c r="H43">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-32.098540072895489</v>
+        <v>-34.906511598055907</v>
       </c>
       <c r="I43" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.64197080145790975</v>
+        <v>0.69813023196111812</v>
       </c>
       <c r="J43">
         <v>2</v>
@@ -2959,7 +2959,7 @@
         <v>1.5708</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M43">
         <v>14</v>
@@ -2973,51 +2973,51 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B44">
-        <v>7.8680847462490462</v>
+        <v>5.1033013638037135</v>
       </c>
       <c r="C44">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>6.1319152537509538</v>
+        <v>8.8966986361962874</v>
       </c>
       <c r="D44" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.43799394669649672</v>
+        <v>0.63547847401402058</v>
       </c>
       <c r="E44">
-        <v>0.35481923329909559</v>
+        <v>1.4471195362592375</v>
       </c>
       <c r="F44">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.35481923329909559</v>
+        <v>0.12368046374076247</v>
       </c>
       <c r="G44">
-        <v>-16.87791579408179</v>
+        <v>-24.283291971437549</v>
       </c>
       <c r="H44">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-33.122084205918213</v>
+        <v>-25.716708028562451</v>
       </c>
       <c r="I44" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.66244168411836424</v>
+        <v>0.51433416057124903</v>
       </c>
       <c r="J44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K44">
-        <v>3.1415999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M44">
         <v>14</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>1.5708</v>
       </c>
       <c r="O44">
         <v>-50</v>
@@ -3025,51 +3025,51 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B45">
-        <v>6.6592866623578741</v>
+        <v>4.4914514413503923</v>
       </c>
       <c r="C45">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>7.3407133376421259</v>
+        <v>9.5085485586496077</v>
       </c>
       <c r="D45" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.52433666697443759</v>
+        <v>0.67918203990354342</v>
       </c>
       <c r="E45">
-        <v>0.33923882984389042</v>
+        <v>2.2673247983384548</v>
       </c>
       <c r="F45">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.33923882984389042</v>
+        <v>8.8875201661545056E-2</v>
       </c>
       <c r="G45">
-        <v>-23.46730562987506</v>
+        <v>-5.8876235417411715</v>
       </c>
       <c r="H45">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.53269437012494</v>
+        <v>-44.112376458258829</v>
       </c>
       <c r="I45" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.53065388740249875</v>
+        <v>0.88224752916517657</v>
       </c>
       <c r="J45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K45">
         <v>1.5708</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M45">
         <v>14</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O45">
         <v>-50</v>
@@ -3077,51 +3077,51 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="B46">
-        <v>6.3743981072779015</v>
+        <v>4.2039063534328456</v>
       </c>
       <c r="C46">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>7.6256018927220985</v>
+        <v>9.7960936465671544</v>
       </c>
       <c r="D46" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.54468584948014986</v>
+        <v>0.69972097475479678</v>
       </c>
       <c r="E46">
-        <v>0.30915273724810233</v>
+        <v>1.7948297539227032</v>
       </c>
       <c r="F46">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.30915273724810233</v>
+        <v>-0.22402975392270319</v>
       </c>
       <c r="G46">
-        <v>-22.557797164235772</v>
+        <v>-7.3471574467405381</v>
       </c>
       <c r="H46">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-27.442202835764228</v>
+        <v>-42.652842553259461</v>
       </c>
       <c r="I46" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.54884405671528458</v>
+        <v>0.85305685106518925</v>
       </c>
       <c r="J46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K46">
-        <v>3.1415999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M46">
         <v>14</v>
       </c>
       <c r="N46">
-        <v>0</v>
+        <v>1.5708</v>
       </c>
       <c r="O46">
         <v>-50</v>
@@ -3129,36 +3129,36 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B47">
-        <v>6.1663487885469292</v>
+        <v>4.0881215575992274</v>
       </c>
       <c r="C47">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>7.8336512114530708</v>
+        <v>9.9118784424007735</v>
       </c>
       <c r="D47" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.55954651510379072</v>
+        <v>0.70799131731434095</v>
       </c>
       <c r="E47">
-        <v>1.2764813931533183</v>
+        <v>2.3464366793412288</v>
       </c>
       <c r="F47">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0.29431860684668165</v>
+        <v>9.7633206587710575E-3</v>
       </c>
       <c r="G47">
-        <v>-23.499896278221737</v>
+        <v>-13.104123864074159</v>
       </c>
       <c r="H47">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.500103721778263</v>
+        <v>-36.895876135925839</v>
       </c>
       <c r="I47" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.53000207443556524</v>
+        <v>0.73791752271851674</v>
       </c>
       <c r="J47">
         <v>3</v>
@@ -3167,13 +3167,13 @@
         <v>1.5708</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M47">
         <v>14</v>
       </c>
       <c r="N47">
-        <v>1.5708</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O47">
         <v>-50</v>
@@ -3181,51 +3181,51 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B48">
-        <v>5.1033013638037135</v>
+        <v>10.499308160078709</v>
       </c>
       <c r="C48">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>8.8966986361962874</v>
+        <v>3.5006918399212914</v>
       </c>
       <c r="D48" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.63547847401402058</v>
+        <v>0.25004941713723511</v>
       </c>
       <c r="E48">
-        <v>1.4471195362592375</v>
+        <v>0.89441113446496479</v>
       </c>
       <c r="F48">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0.12368046374076247</v>
+        <v>-0.1090111344649648</v>
       </c>
       <c r="G48">
-        <v>-24.283291971437549</v>
+        <v>-24.439339774013547</v>
       </c>
       <c r="H48">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-25.716708028562451</v>
+        <v>-25.560660225986453</v>
       </c>
       <c r="I48" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.51433416057124903</v>
+        <v>0.51121320451972907</v>
       </c>
       <c r="J48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K48">
         <v>1.5708</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M48">
         <v>14</v>
       </c>
       <c r="N48">
-        <v>1.5708</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O48">
         <v>-50</v>
@@ -3233,51 +3233,51 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>10.125292754787109</v>
+      </c>
+      <c r="C49">
+        <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
+        <v>3.8747072452128908</v>
+      </c>
+      <c r="D49" s="3">
+        <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
+        <v>0.27676480322949221</v>
+      </c>
+      <c r="E49">
+        <v>0.94899438432264316</v>
+      </c>
+      <c r="F49">
+        <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
+        <v>-0.16359438432264317</v>
+      </c>
+      <c r="G49">
+        <v>-30.869370476054289</v>
+      </c>
+      <c r="H49">
+        <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
+        <v>-19.130629523945711</v>
+      </c>
+      <c r="I49" s="3">
+        <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
+        <v>0.38261259047891422</v>
+      </c>
+      <c r="J49">
         <v>3</v>
       </c>
-      <c r="B49">
-        <v>5.043608780281355</v>
-      </c>
-      <c r="C49">
-        <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>8.956391219718645</v>
-      </c>
-      <c r="D49" s="3">
-        <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.63974222997990327</v>
-      </c>
-      <c r="E49">
-        <v>1.6178626419664945</v>
-      </c>
-      <c r="F49">
-        <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-4.7062641966494567E-2</v>
-      </c>
-      <c r="G49">
-        <v>-17.920526461740312</v>
-      </c>
-      <c r="H49">
-        <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-32.079473538259691</v>
-      </c>
-      <c r="I49" s="3">
-        <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.64158947076519379</v>
-      </c>
-      <c r="J49">
-        <v>2</v>
-      </c>
       <c r="K49">
         <v>1.5708</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M49">
         <v>14</v>
       </c>
       <c r="N49">
-        <v>1.5708</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O49">
         <v>-50</v>
@@ -3285,36 +3285,36 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B50">
-        <v>5.043608780281355</v>
+        <v>9.6783889588051313</v>
       </c>
       <c r="C50">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>8.956391219718645</v>
+        <v>4.3216110411948687</v>
       </c>
       <c r="D50" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.63974222997990327</v>
+        <v>0.30868650294249061</v>
       </c>
       <c r="E50">
-        <v>1.6178626419664945</v>
+        <v>0.63668707506666289</v>
       </c>
       <c r="F50">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-4.7062641966494567E-2</v>
+        <v>-0.63668707506666289</v>
       </c>
       <c r="G50">
-        <v>-17.920526461740312</v>
+        <v>-20.806605765438739</v>
       </c>
       <c r="H50">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-32.079473538259691</v>
+        <v>-29.193394234561261</v>
       </c>
       <c r="I50" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.64158947076519379</v>
+        <v>0.58386788469122519</v>
       </c>
       <c r="J50">
         <v>2</v>
@@ -3329,7 +3329,7 @@
         <v>14</v>
       </c>
       <c r="N50">
-        <v>1.5708</v>
+        <v>0</v>
       </c>
       <c r="O50">
         <v>-50</v>
@@ -3337,51 +3337,51 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B51">
-        <v>4.4932513513810193</v>
+        <v>9.5564130488735231</v>
       </c>
       <c r="C51">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>9.5067486486189807</v>
+        <v>4.4435869511264769</v>
       </c>
       <c r="D51" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.67905347490135581</v>
+        <v>0.31739906793760547</v>
       </c>
       <c r="E51">
-        <v>1.4973105497117114</v>
+        <v>0.62560324580990911</v>
       </c>
       <c r="F51">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>7.3489450288288571E-2</v>
+        <v>-0.62560324580990911</v>
       </c>
       <c r="G51">
-        <v>-23.551161455515949</v>
+        <v>-19.474191154986151</v>
       </c>
       <c r="H51">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-26.448838544484051</v>
+        <v>-30.525808845013849</v>
       </c>
       <c r="I51" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.52897677088968098</v>
+        <v>0.61051617690027693</v>
       </c>
       <c r="J51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K51">
-        <v>1.5708</v>
+        <v>3.1415999999999999</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M51">
         <v>14</v>
       </c>
       <c r="N51">
-        <v>1.5708</v>
+        <v>0</v>
       </c>
       <c r="O51">
         <v>-50</v>
@@ -3389,39 +3389,39 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B52">
-        <v>4.4914514413503923</v>
+        <v>8.3886643956393581</v>
       </c>
       <c r="C52">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>9.5085485586496077</v>
+        <v>5.6113356043606419</v>
       </c>
       <c r="D52" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.67918203990354342</v>
+        <v>0.40080968602576011</v>
       </c>
       <c r="E52">
-        <v>2.2673247983384548</v>
+        <v>0.38018833531851759</v>
       </c>
       <c r="F52">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>8.8875201661545056E-2</v>
+        <v>-0.38018833531851759</v>
       </c>
       <c r="G52">
-        <v>-5.8876235417411715</v>
+        <v>-23.591162741785809</v>
       </c>
       <c r="H52">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-44.112376458258829</v>
+        <v>-26.408837258214191</v>
       </c>
       <c r="I52" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.88224752916517657</v>
+        <v>0.52817674516428381</v>
       </c>
       <c r="J52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K52">
         <v>1.5708</v>
@@ -3433,7 +3433,7 @@
         <v>14</v>
       </c>
       <c r="N52">
-        <v>2.3561999999999999</v>
+        <v>0</v>
       </c>
       <c r="O52">
         <v>-50</v>
@@ -3441,51 +3441,51 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B53">
-        <v>4.4914514413503923</v>
+        <v>6.1663487885469292</v>
       </c>
       <c r="C53">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>9.5085485586496077</v>
+        <v>7.8336512114530708</v>
       </c>
       <c r="D53" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.67918203990354342</v>
+        <v>0.55954651510379072</v>
       </c>
       <c r="E53">
-        <v>2.2673247983384548</v>
+        <v>1.2764813931533183</v>
       </c>
       <c r="F53">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>8.8875201661545056E-2</v>
+        <v>0.29431860684668165</v>
       </c>
       <c r="G53">
-        <v>-5.8876235417411715</v>
+        <v>-23.499896278221737</v>
       </c>
       <c r="H53">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-44.112376458258829</v>
+        <v>-26.500103721778263</v>
       </c>
       <c r="I53" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.88224752916517657</v>
+        <v>0.53000207443556524</v>
       </c>
       <c r="J53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K53">
         <v>1.5708</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M53">
         <v>14</v>
       </c>
       <c r="N53">
-        <v>2.3561999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="O53">
         <v>-50</v>
@@ -3493,36 +3493,36 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B54">
-        <v>4.2039063534328456</v>
+        <v>5.043608780281355</v>
       </c>
       <c r="C54">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>9.7960936465671544</v>
+        <v>8.956391219718645</v>
       </c>
       <c r="D54" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.69972097475479678</v>
+        <v>0.63974222997990327</v>
       </c>
       <c r="E54">
-        <v>1.7948297539227032</v>
+        <v>1.6178626419664945</v>
       </c>
       <c r="F54">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.22402975392270319</v>
+        <v>-4.7062641966494567E-2</v>
       </c>
       <c r="G54">
-        <v>-7.3471574467405381</v>
+        <v>-17.920526461740312</v>
       </c>
       <c r="H54">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-42.652842553259461</v>
+        <v>-32.079473538259691</v>
       </c>
       <c r="I54" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.85305685106518925</v>
+        <v>0.64158947076519379</v>
       </c>
       <c r="J54">
         <v>2</v>
@@ -3531,7 +3531,7 @@
         <v>1.5708</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M54">
         <v>14</v>
@@ -3545,45 +3545,45 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B55">
-        <v>4.0881215575992274</v>
+        <v>4.4914514413503923</v>
       </c>
       <c r="C55">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>9.9118784424007735</v>
+        <v>9.5085485586496077</v>
       </c>
       <c r="D55" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.70799131731434095</v>
+        <v>0.67918203990354342</v>
       </c>
       <c r="E55">
-        <v>2.3464366793412288</v>
+        <v>2.2673247983384548</v>
       </c>
       <c r="F55">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>9.7633206587710575E-3</v>
+        <v>8.8875201661545056E-2</v>
       </c>
       <c r="G55">
-        <v>-13.104123864074159</v>
+        <v>-5.8876235417411715</v>
       </c>
       <c r="H55">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-36.895876135925839</v>
+        <v>-44.112376458258829</v>
       </c>
       <c r="I55" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.73791752271851674</v>
+        <v>0.88224752916517657</v>
       </c>
       <c r="J55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K55">
         <v>1.5708</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M55">
         <v>14</v>
@@ -3597,45 +3597,45 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="B56">
-        <v>3.4000339721819084</v>
+        <v>3.335356272803502</v>
       </c>
       <c r="C56">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>10.599966027818091</v>
+        <v>10.664643727196498</v>
       </c>
       <c r="D56" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.75714043055843505</v>
+        <v>0.76176026622832127</v>
       </c>
       <c r="E56">
-        <v>2.3563215470535948</v>
+        <v>2.3590384677248712</v>
       </c>
       <c r="F56">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-1.2154705359490592E-4</v>
+        <v>-2.8384677248713963E-3</v>
       </c>
       <c r="G56">
-        <v>-2.8961799755479558</v>
+        <v>-17.639696982700809</v>
       </c>
       <c r="H56">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-47.103820024452041</v>
+        <v>-32.360303017299188</v>
       </c>
       <c r="I56" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.94207640048904084</v>
+        <v>0.64720606034598371</v>
       </c>
       <c r="J56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K56">
         <v>1.5708</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M56">
         <v>14</v>
@@ -3649,51 +3649,51 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B57">
-        <v>3.335356272803502</v>
+        <v>10.585348818604754</v>
       </c>
       <c r="C57">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>10.664643727196498</v>
+        <v>3.4146511813952465</v>
       </c>
       <c r="D57" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.76176026622832127</v>
+        <v>0.24390365581394619</v>
       </c>
       <c r="E57">
-        <v>2.3590384677248712</v>
+        <v>0.91317589587935233</v>
       </c>
       <c r="F57">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-2.8384677248713963E-3</v>
+        <v>-0.12777589587935234</v>
       </c>
       <c r="G57">
-        <v>-17.639696982700809</v>
+        <v>-24.753182054066464</v>
       </c>
       <c r="H57">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-32.360303017299188</v>
+        <v>-25.246817945933536</v>
       </c>
       <c r="I57" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.64720606034598371</v>
+        <v>0.50493635891867072</v>
       </c>
       <c r="J57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K57">
         <v>1.5708</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="M57">
         <v>14</v>
       </c>
       <c r="N57">
-        <v>2.3561999999999999</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O57">
         <v>-50</v>
@@ -3701,51 +3701,51 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B58">
-        <v>3.335356272803502</v>
+        <v>10.585348818604754</v>
       </c>
       <c r="C58">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>10.664643727196498</v>
+        <v>3.4146511813952465</v>
       </c>
       <c r="D58" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.76176026622832127</v>
+        <v>0.24390365581394619</v>
       </c>
       <c r="E58">
-        <v>2.3590384677248712</v>
+        <v>0.91317589587935233</v>
       </c>
       <c r="F58">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-2.8384677248713963E-3</v>
+        <v>-0.91317589587935233</v>
       </c>
       <c r="G58">
-        <v>-17.639696982700809</v>
+        <v>-24.753182054066464</v>
       </c>
       <c r="H58">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-32.360303017299188</v>
+        <v>-25.246817945933536</v>
       </c>
       <c r="I58" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.64720606034598371</v>
+        <v>0.50493635891867072</v>
       </c>
       <c r="J58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K58">
         <v>1.5708</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M58">
         <v>14</v>
       </c>
       <c r="N58">
-        <v>2.3561999999999999</v>
+        <v>0</v>
       </c>
       <c r="O58">
         <v>-50</v>
@@ -3753,51 +3753,51 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B59">
-        <v>2.744578901867996</v>
+        <v>10.585348818604754</v>
       </c>
       <c r="C59">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>11.255421098132004</v>
+        <v>3.4146511813952465</v>
       </c>
       <c r="D59" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.80395864986657173</v>
+        <v>0.24390365581394619</v>
       </c>
       <c r="E59">
-        <v>0.80803646616466207</v>
+        <v>0.91317589587935233</v>
       </c>
       <c r="F59">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-2.2636466164662084E-2</v>
+        <v>0.65762410412064765</v>
       </c>
       <c r="G59">
-        <v>-10.201235887648528</v>
+        <v>-24.753182054066464</v>
       </c>
       <c r="H59">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-39.798764112351471</v>
+        <v>-25.246817945933536</v>
       </c>
       <c r="I59" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.7959752822470294</v>
+        <v>0.50493635891867072</v>
       </c>
       <c r="J59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K59">
         <v>1.5708</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M59">
         <v>14</v>
       </c>
       <c r="N59">
-        <v>0.78539999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="O59">
         <v>-50</v>
@@ -3805,36 +3805,36 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B60">
-        <v>2.5142693426197287</v>
+        <v>10.585348818604754</v>
       </c>
       <c r="C60">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>11.485730657380271</v>
+        <v>3.4146511813952465</v>
       </c>
       <c r="D60" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.82040933267001936</v>
+        <v>0.24390365581394619</v>
       </c>
       <c r="E60">
-        <v>0.78509778249465201</v>
+        <v>0.91317589587935233</v>
       </c>
       <c r="F60">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>3.022175053479792E-4</v>
+        <v>1.4430241041206475</v>
       </c>
       <c r="G60">
-        <v>-5.8806851197080983</v>
+        <v>-24.753182054066464</v>
       </c>
       <c r="H60">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-44.119314880291903</v>
+        <v>-25.246817945933536</v>
       </c>
       <c r="I60" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.88238629760583809</v>
+        <v>0.50493635891867072</v>
       </c>
       <c r="J60">
         <v>2</v>
@@ -3843,13 +3843,13 @@
         <v>1.5708</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M60">
         <v>14</v>
       </c>
       <c r="N60">
-        <v>0.78539999999999999</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O60">
         <v>-50</v>
@@ -3857,51 +3857,51 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B61">
-        <v>2.401507748371428</v>
+        <v>10.552836725047491</v>
       </c>
       <c r="C61">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>11.598492251628572</v>
+        <v>3.4471632749525085</v>
       </c>
       <c r="D61" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.82846373225918379</v>
+        <v>0.24622594821089347</v>
       </c>
       <c r="E61">
-        <v>2.5655023310780454</v>
+        <v>1.0891326578930076</v>
       </c>
       <c r="F61">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-0.20930233107804552</v>
+        <v>-1.0891326578930076</v>
       </c>
       <c r="G61">
-        <v>-2.191225676254779</v>
+        <v>-29.429198612896048</v>
       </c>
       <c r="H61">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-47.808774323745219</v>
+        <v>-20.570801387103952</v>
       </c>
       <c r="I61" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.95617548647490436</v>
+        <v>0.41141602774207903</v>
       </c>
       <c r="J61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K61">
-        <v>1.5708</v>
+        <v>3.1415999999999999</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="M61">
         <v>14</v>
       </c>
       <c r="N61">
-        <v>2.3561999999999999</v>
+        <v>0</v>
       </c>
       <c r="O61">
         <v>-50</v>
@@ -3909,51 +3909,51 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B62">
-        <v>0.60485634565557433</v>
+        <v>10.357264128043649</v>
       </c>
       <c r="C62">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>13.395143654344425</v>
+        <v>3.6427358719563507</v>
       </c>
       <c r="D62" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.95679597531031602</v>
+        <v>0.2601954194254536</v>
       </c>
       <c r="E62">
-        <v>1.5710418429033823</v>
+        <v>1.0156881149436505</v>
       </c>
       <c r="F62">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-2.4184290338236103E-4</v>
+        <v>-1.0156881149436505</v>
       </c>
       <c r="G62">
-        <v>-1.1473067014842466</v>
+        <v>-24.689535971972997</v>
       </c>
       <c r="H62">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-48.852693298515753</v>
+        <v>-25.310464028027003</v>
       </c>
       <c r="I62" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.97705386597031507</v>
+        <v>0.50620928056054004</v>
       </c>
       <c r="J62">
         <v>2</v>
       </c>
       <c r="K62">
-        <v>1.5708</v>
+        <v>3.1415999999999999</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M62">
         <v>14</v>
       </c>
       <c r="N62">
-        <v>1.5708</v>
+        <v>0</v>
       </c>
       <c r="O62">
         <v>-50</v>
@@ -3961,36 +3961,36 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B63">
-        <v>0.5430226005706229</v>
+        <v>10.352459970417151</v>
       </c>
       <c r="C63">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>13.456977399429377</v>
+        <v>3.6475400295828493</v>
       </c>
       <c r="D63" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.96121267138781263</v>
+        <v>0.26053857354163207</v>
       </c>
       <c r="E63">
-        <v>1.1904643963441685E-4</v>
+        <v>1.0503872048170404</v>
       </c>
       <c r="F63">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>-1.1904643963441685E-4</v>
+        <v>-0.26498720481704041</v>
       </c>
       <c r="G63">
-        <v>0.19305650313308748</v>
+        <v>-31.214827041527919</v>
       </c>
       <c r="H63">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-50.193056503133086</v>
+        <v>-18.785172958472081</v>
       </c>
       <c r="I63" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>1.0038611300626616</v>
+        <v>0.37570345916944164</v>
       </c>
       <c r="J63">
         <v>3</v>
@@ -3999,13 +3999,13 @@
         <v>1.5708</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M63">
         <v>14</v>
       </c>
       <c r="N63">
-        <v>0</v>
+        <v>0.78539999999999999</v>
       </c>
       <c r="O63">
         <v>-50</v>
@@ -4013,36 +4013,36 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B64">
-        <v>0.22599794935528578</v>
+        <v>10.352459970417151</v>
       </c>
       <c r="C64">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>13.774002050644715</v>
+        <v>3.6475400295828493</v>
       </c>
       <c r="D64" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.98385728933176531</v>
+        <v>0.26053857354163207</v>
       </c>
       <c r="E64">
-        <v>1.570281885757705</v>
+        <v>1.0503872048170404</v>
       </c>
       <c r="F64">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>5.1811424229497582E-4</v>
+        <v>-1.0503872048170404</v>
       </c>
       <c r="G64">
-        <v>-0.88538910829364359</v>
+        <v>-31.214827041527919</v>
       </c>
       <c r="H64">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-49.114610891706356</v>
+        <v>-18.785172958472081</v>
       </c>
       <c r="I64" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.98229221783412712</v>
+        <v>0.37570345916944164</v>
       </c>
       <c r="J64">
         <v>3</v>
@@ -4051,13 +4051,13 @@
         <v>1.5708</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M64">
         <v>14</v>
       </c>
       <c r="N64">
-        <v>1.5708</v>
+        <v>0</v>
       </c>
       <c r="O64">
         <v>-50</v>
@@ -4065,36 +4065,36 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B65">
-        <v>2.1593038339367231E-2</v>
+        <v>10.352459970417151</v>
       </c>
       <c r="C65">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>13.978406961660633</v>
+        <v>3.6475400295828493</v>
       </c>
       <c r="D65" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>0.99845764011861671</v>
+        <v>0.26053857354163207</v>
       </c>
       <c r="E65">
-        <v>2.3355974509498942</v>
+        <v>1.0503872048170404</v>
       </c>
       <c r="F65">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>2.0602549050105612E-2</v>
+        <v>0.52041279518295958</v>
       </c>
       <c r="G65">
-        <v>-0.3560193649975919</v>
+        <v>-31.214827041527919</v>
       </c>
       <c r="H65">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-49.643980635002407</v>
+        <v>-18.785172958472081</v>
       </c>
       <c r="I65" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>0.9928796127000481</v>
+        <v>0.37570345916944164</v>
       </c>
       <c r="J65">
         <v>3</v>
@@ -4103,13 +4103,13 @@
         <v>1.5708</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M65">
         <v>14</v>
       </c>
       <c r="N65">
-        <v>2.3561999999999999</v>
+        <v>1.5708</v>
       </c>
       <c r="O65">
         <v>-50</v>
@@ -4117,51 +4117,51 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>10.352459970417151</v>
       </c>
       <c r="C66">
         <f>Table1[[#This Row],[Vel Goal]]-Table1[[#This Row],[Velocity]]</f>
-        <v>14</v>
+        <v>3.6475400295828493</v>
       </c>
       <c r="D66" s="3">
         <f>Table1[[#This Row],[Velocity error]]/Table1[[#This Row],[Vel Goal]]</f>
-        <v>1</v>
+        <v>0.26053857354163207</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>1.0503872048170404</v>
       </c>
       <c r="F66">
         <f>Table1[[#This Row],[Ang Goal]]-Table1[[#This Row],[Angle]]</f>
-        <v>0</v>
+        <v>1.3058127951829595</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>-31.214827041527919</v>
       </c>
       <c r="H66">
         <f>Table1[[#This Row],[Spin Goal]]-Table1[[#This Row],[Spin]]</f>
-        <v>-50</v>
+        <v>-18.785172958472081</v>
       </c>
       <c r="I66" s="3">
         <f>Table1[[#This Row],[Spin Error]]/Table1[[#This Row],[Spin Goal]]</f>
-        <v>1</v>
+        <v>0.37570345916944164</v>
       </c>
       <c r="J66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K66">
         <v>1.5708</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M66">
         <v>14</v>
       </c>
       <c r="N66">
-        <v>0</v>
+        <v>2.3561999999999999</v>
       </c>
       <c r="O66">
         <v>-50</v>

</xml_diff>